<commit_message>
make table in readme.md
</commit_message>
<xml_diff>
--- a/README_img/readme_img.xlsx
+++ b/README_img/readme_img.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teramoto\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teramoto\Desktop\git\Proteins_NER\README_img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB8292B-B36B-4C7E-9AD9-4D7A06A53EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF50A970-9099-4C4F-B639-D5EDFC69D656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10560" xr2:uid="{D7B59021-8C94-44A2-83B3-CB0BADFC5260}"/>
+    <workbookView xWindow="3430" yWindow="-9270" windowWidth="12340" windowHeight="5970" xr2:uid="{D7B59021-8C94-44A2-83B3-CB0BADFC5260}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>bioinfer</t>
   </si>
   <si>
-    <t>aimed</t>
-  </si>
-  <si>
     <t>合計</t>
     <rPh sb="0" eb="2">
       <t>ゴウケイ</t>
@@ -90,6 +87,10 @@
     <rPh sb="2" eb="4">
       <t>ケッカ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aimed</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -578,7 +579,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$3</c15:sqref>
@@ -610,7 +611,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000001-0000-44DC-B007-6D52EA7F8846}"/>
                     </c:ext>
@@ -630,7 +631,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000003-0000-44DC-B007-6D52EA7F8846}"/>
                     </c:ext>
@@ -650,7 +651,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000005-0000-44DC-B007-6D52EA7F8846}"/>
                     </c:ext>
@@ -670,7 +671,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000007-0000-44DC-B007-6D52EA7F8846}"/>
                     </c:ext>
@@ -678,7 +679,7 @@
                 </c:dPt>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1:$E$1</c15:sqref>
@@ -704,7 +705,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$3:$E$3</c15:sqref>
@@ -729,7 +730,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-0000-44DC-B007-6D52EA7F8846}"/>
                   </c:ext>
@@ -10852,8 +10853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A1E342-1776-4C09-B3DB-88286C8EC086}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
@@ -10867,10 +10868,10 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -10879,12 +10880,12 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>642</v>

</xml_diff>